<commit_message>
Some change in Q&A file
</commit_message>
<xml_diff>
--- a/Q&A.xlsx
+++ b/Q&A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\OneDrive\Máy tính\TVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55343ECC-6C81-4DAA-A588-A458C156ABF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364A220C-C44A-48BC-894A-C091DFA0D84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12735" yWindow="0" windowWidth="16035" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -26,76 +26,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>1. What type of front-end should this system have?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Winform</t>
   </si>
   <si>
-    <t>2. Which data will be stored?</t>
-  </si>
-  <si>
-    <t>1. Which ticket does this machine sell?</t>
-  </si>
-  <si>
-    <t>Bus ticket</t>
-  </si>
-  <si>
-    <t>2. What kind of ticket (one-way, two-way)?</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>3. What type of payment options will the TVM support?</t>
-  </si>
-  <si>
-    <t>Credit/ debit card and mobile payments (using QR code)</t>
-  </si>
-  <si>
-    <t>Destinations (Bus stop, routes, …)</t>
-  </si>
-  <si>
-    <t>4. What will help users to plan their trips?</t>
-  </si>
-  <si>
-    <t>5. Who will use this TVM?</t>
-  </si>
-  <si>
-    <t>It will have a schedule and routes of each available bus displayed</t>
-  </si>
-  <si>
-    <t>6. How TVM can validate card transactions?</t>
-  </si>
-  <si>
-    <t>Integrated with banking system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banking system </t>
-  </si>
-  <si>
-    <t>Digital wallet</t>
-  </si>
-  <si>
-    <t>Logs of transactions</t>
-  </si>
-  <si>
-    <t>3. Where the data will be stored?</t>
-  </si>
-  <si>
-    <t>MSSQL database</t>
-  </si>
-  <si>
-    <t>Customer, operator</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>What is the purpose of the TVM?</t>
+  </si>
+  <si>
+    <t>This TVM is an automated ticket-issuing system for public transportation.</t>
+  </si>
+  <si>
+    <t>Credit/debit card, QR code payment linked with banking system or digital wallet.</t>
+  </si>
+  <si>
+    <t>What payment modes are available for the users?</t>
+  </si>
+  <si>
+    <t>The TVM issues a paper ticket with a bar code and their card account is charged.</t>
+  </si>
+  <si>
+    <t>The TVM shows a QR code to the user. Once transaction is finished, the TVM will issues a paper ticket with a bar code.</t>
+  </si>
+  <si>
+    <t>The TVM will calculate and show the ticket price to the user base on each type of available mode of transportations.</t>
+  </si>
+  <si>
+    <t>What happens after a user select their destination?</t>
+  </si>
+  <si>
+    <t>What happens when a user select credit/debit card payment option?</t>
+  </si>
+  <si>
+    <t>What happens when a user select digital wallet payment option?</t>
+  </si>
+  <si>
+    <t>What happens after a user select their desired mode of transportation?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They are requested to chose one of the available payment modes. </t>
+  </si>
+  <si>
+    <t>What language does the TVM support?</t>
+  </si>
+  <si>
+    <t>Vietnamese and English</t>
+  </si>
+  <si>
+    <t>Who will use the TVM?</t>
+  </si>
+  <si>
+    <t>Customer and operator</t>
+  </si>
+  <si>
+    <t>What type of front-end should the TVM have?</t>
+  </si>
+  <si>
+    <t>What type of data will be stored?</t>
+  </si>
+  <si>
+    <t>Destination, transaction logs, information related to banking system and digital wallet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,16 +109,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -120,17 +152,240 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -141,6 +396,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5AA96FA0-A9CE-45CB-9E3F-18172EDCC0AF}" name="Table33" displayName="Table33" ref="B2:D7" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B2:D7" xr:uid="{5AA96FA0-A9CE-45CB-9E3F-18172EDCC0AF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{7E9A33AC-1B01-4593-A264-08975CF9E49A}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{3F50B491-64D3-4AB3-8110-FC1869B923FD}" name="Question" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{E906C5C8-C091-4104-9D57-A2DAB192B61E}" name="Answer" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,104 +687,216 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="3" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K7" t="s">
+    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some change in the usecase diagram and add descriptions to 3/6 usecase
</commit_message>
<xml_diff>
--- a/Q&A.xlsx
+++ b/Q&A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\OneDrive\Máy tính\TVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA7D8CD-5BAC-4933-912A-4C137F0DB54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F45FC30-1344-4696-9EEB-A3673E978ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>The TVM issues a paper ticket with a bar code and their card account is charged.</t>
   </si>
   <si>
-    <t>The TVM shows a QR code to the user. Once transaction is finished, the TVM will issues a paper ticket with a bar code.</t>
-  </si>
-  <si>
     <t>What happens after a user select their destination?</t>
   </si>
   <si>
@@ -99,7 +96,10 @@
     <t>What happens after a user submits their selection?</t>
   </si>
   <si>
-    <t>Destination, transaction logs, information related to banking systems and digital wallets</t>
+    <t>The TVM shows a QR code to the user. Once the transaction is finished, the TVM will issues a paper ticket with a bar code.</t>
+  </si>
+  <si>
+    <t>Destination, transaction logs, error logs, customer feedbacks, information related to banking systems and digital wallets</t>
   </si>
 </sst>
 </file>
@@ -801,17 +801,17 @@
   <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="58.140625" customWidth="1"/>
-    <col min="4" max="4" width="65.28515625" customWidth="1"/>
+    <col min="3" max="3" width="58.109375" customWidth="1"/>
+    <col min="4" max="4" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -822,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="12">
         <v>1</v>
       </c>
@@ -830,10 +830,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B4" s="13">
         <v>2</v>
       </c>
@@ -844,100 +844,100 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="51.75" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="52.2" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B7" s="13">
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B8" s="14">
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="17.25" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" s="18" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:4" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B12" s="14">
         <v>10</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Finish activity, sequence, statechart, usecase diagram. Maybe updated later
</commit_message>
<xml_diff>
--- a/Q&A.xlsx
+++ b/Q&A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\OneDrive\Máy tính\TVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F45FC30-1344-4696-9EEB-A3673E978ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8906865C-601E-446B-A32D-95B7178E70EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>What is the purpose of the TVM?</t>
   </si>
   <si>
-    <t>Credit/debit card, QR code payment linked with banking system or digital wallet.</t>
-  </si>
-  <si>
     <t>What payment modes are available for the users?</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>What happens after a user select their destination?</t>
   </si>
   <si>
-    <t>What happens when a user select credit/debit card payment option?</t>
-  </si>
-  <si>
     <t>What happens when a user select digital wallet payment option?</t>
   </si>
   <si>
@@ -84,12 +78,6 @@
     <t>This TVM is an automated ticket-issuing system for MRT.</t>
   </si>
   <si>
-    <t>The TVM displays a menu of available destinations to the user.</t>
-  </si>
-  <si>
-    <t>The TVM calculates and displays the ticket price, as well as allowing the user to choose the quantity of tickets they want to purchase.</t>
-  </si>
-  <si>
     <t>What happens after user hit the start button?</t>
   </si>
   <si>
@@ -99,7 +87,19 @@
     <t>The TVM shows a QR code to the user. Once the transaction is finished, the TVM will issues a paper ticket with a bar code.</t>
   </si>
   <si>
-    <t>Destination, transaction logs, error logs, customer feedbacks, information related to banking systems and digital wallets</t>
+    <t>Destination, transaction log, error log, customer feedbacks, information related to banking systems and digital wallets</t>
+  </si>
+  <si>
+    <t>ATM card, QR code payment linked with banking system or digital wallet.</t>
+  </si>
+  <si>
+    <t>What happens when a user select ATM card payment option?</t>
+  </si>
+  <si>
+    <t>The TVM displays a menu of available destinations together with the price to the user.</t>
+  </si>
+  <si>
+    <t>The user chooses the quantity of tickets they want to purchase.</t>
   </si>
 </sst>
 </file>
@@ -801,17 +801,17 @@
   <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="58.109375" customWidth="1"/>
-    <col min="4" max="4" width="65.33203125" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -822,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B3" s="12">
         <v>1</v>
       </c>
@@ -830,117 +830,117 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B4" s="13">
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="52.2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B7" s="13">
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B10" s="14">
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" s="18" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B12" s="14">
         <v>10</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>